<commit_message>
Updating Excel Modification Code + Cucumber Features
</commit_message>
<xml_diff>
--- a/Happle Mind/TestscriptManager/TestscriptManager.xlsx
+++ b/Happle Mind/TestscriptManager/TestscriptManager.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="11025" windowHeight="6090" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11025" windowHeight="6090"/>
   </bookViews>
   <sheets>
     <sheet name="Set 1" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>Set 2 Test scenario 5</t>
   </si>
   <si>
-    <t>Set 1 Test case 1</t>
-  </si>
-  <si>
     <t>Set 1 Test case 2</t>
   </si>
   <si>
@@ -87,6 +84,9 @@
   </si>
   <si>
     <t>Set 1 Test scenario 5</t>
+  </si>
+  <si>
+    <t>TC1</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,13 +480,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -494,10 +494,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -508,13 +508,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -522,13 +522,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -536,10 +536,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -559,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +612,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -654,7 +654,7 @@
         <v>13</v>
       </c>
       <c r="D6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>